<commit_message>
Add BAA years to main data
</commit_message>
<xml_diff>
--- a/NBASeriesML/NBASeriesResults.xlsx
+++ b/NBASeriesML/NBASeriesResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usolon\Documents\NBASeriesML\NBASeriesML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60876231-787C-4EDC-9859-E584B0673B1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE4496D-5D83-4D4C-8F78-408A7336ADDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{E5EB9399-3DE7-464A-8398-E490882B2270}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6644" uniqueCount="1322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6644" uniqueCount="1324">
   <si>
     <t>Year</t>
   </si>
@@ -4006,6 +4006,12 @@
   </si>
   <si>
     <t>Memphis Sounds</t>
+  </si>
+  <si>
+    <t>St. Louis Bombers</t>
+  </si>
+  <si>
+    <t>Cleveland Rebels</t>
   </si>
 </sst>
 </file>
@@ -35672,8 +35678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDB2D06D-6BBD-46A2-823D-1E442DB84DAE}">
   <dimension ref="A1:U953"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A704" workbookViewId="0">
-      <selection activeCell="A718" sqref="A718:U721"/>
+    <sheetView tabSelected="1" topLeftCell="A936" workbookViewId="0">
+      <selection activeCell="C953" sqref="C953:U953"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -85942,19 +85948,37 @@
         <v>930</v>
       </c>
       <c r="C937" t="s">
-        <v>308</v>
+        <v>1143</v>
       </c>
       <c r="D937">
         <v>2</v>
       </c>
       <c r="E937" t="s">
-        <v>969</v>
+        <v>1228</v>
       </c>
       <c r="F937">
         <v>1</v>
       </c>
       <c r="G937">
         <v>3</v>
+      </c>
+      <c r="H937">
+        <v>81</v>
+      </c>
+      <c r="I937">
+        <v>84</v>
+      </c>
+      <c r="J937">
+        <v>103</v>
+      </c>
+      <c r="O937">
+        <v>82</v>
+      </c>
+      <c r="P937">
+        <v>74</v>
+      </c>
+      <c r="Q937">
+        <v>99</v>
       </c>
     </row>
     <row r="938" spans="1:20" x14ac:dyDescent="0.35">
@@ -85965,19 +85989,31 @@
         <v>930</v>
       </c>
       <c r="C938" t="s">
-        <v>1220</v>
+        <v>1230</v>
       </c>
       <c r="D938">
         <v>2</v>
       </c>
       <c r="E938" t="s">
-        <v>1175</v>
+        <v>1259</v>
       </c>
       <c r="F938">
         <v>0</v>
       </c>
       <c r="G938">
         <v>2</v>
+      </c>
+      <c r="H938">
+        <v>92</v>
+      </c>
+      <c r="I938">
+        <v>80</v>
+      </c>
+      <c r="O938">
+        <v>70</v>
+      </c>
+      <c r="P938">
+        <v>78</v>
       </c>
     </row>
     <row r="939" spans="1:20" x14ac:dyDescent="0.35">
@@ -85988,19 +86024,31 @@
         <v>936</v>
       </c>
       <c r="C939" t="s">
-        <v>1120</v>
+        <v>1133</v>
       </c>
       <c r="D939">
         <v>2</v>
       </c>
       <c r="E939" t="s">
-        <v>1221</v>
+        <v>1196</v>
       </c>
       <c r="F939">
         <v>0</v>
       </c>
       <c r="G939">
         <v>2</v>
+      </c>
+      <c r="H939">
+        <v>84</v>
+      </c>
+      <c r="I939">
+        <v>101</v>
+      </c>
+      <c r="O939">
+        <v>77</v>
+      </c>
+      <c r="P939">
+        <v>85</v>
       </c>
     </row>
     <row r="940" spans="1:20" x14ac:dyDescent="0.35">
@@ -86011,19 +86059,31 @@
         <v>936</v>
       </c>
       <c r="C940" t="s">
-        <v>1179</v>
+        <v>1193</v>
       </c>
       <c r="D940">
         <v>2</v>
       </c>
       <c r="E940" t="s">
-        <v>1223</v>
+        <v>1322</v>
       </c>
       <c r="F940">
         <v>0</v>
       </c>
       <c r="G940">
         <v>2</v>
+      </c>
+      <c r="H940">
+        <v>93</v>
+      </c>
+      <c r="I940">
+        <v>66</v>
+      </c>
+      <c r="O940">
+        <v>64</v>
+      </c>
+      <c r="P940">
+        <v>64</v>
       </c>
     </row>
     <row r="941" spans="1:20" x14ac:dyDescent="0.35">
@@ -86034,19 +86094,37 @@
         <v>940</v>
       </c>
       <c r="C941" t="s">
-        <v>1220</v>
+        <v>1230</v>
       </c>
       <c r="D941">
         <v>2</v>
       </c>
       <c r="E941" t="s">
-        <v>308</v>
+        <v>1143</v>
       </c>
       <c r="F941">
         <v>1</v>
       </c>
       <c r="G941">
         <v>3</v>
+      </c>
+      <c r="H941">
+        <v>77</v>
+      </c>
+      <c r="I941">
+        <v>84</v>
+      </c>
+      <c r="J941">
+        <v>84</v>
+      </c>
+      <c r="O941">
+        <v>71</v>
+      </c>
+      <c r="P941">
+        <v>86</v>
+      </c>
+      <c r="Q941">
+        <v>76</v>
       </c>
     </row>
     <row r="942" spans="1:20" x14ac:dyDescent="0.35">
@@ -86057,19 +86135,31 @@
         <v>983</v>
       </c>
       <c r="C942" t="s">
-        <v>1120</v>
+        <v>1133</v>
       </c>
       <c r="D942">
         <v>2</v>
       </c>
       <c r="E942" t="s">
-        <v>1179</v>
+        <v>1193</v>
       </c>
       <c r="F942">
         <v>0</v>
       </c>
       <c r="G942">
         <v>2</v>
+      </c>
+      <c r="H942">
+        <v>80</v>
+      </c>
+      <c r="I942">
+        <v>67</v>
+      </c>
+      <c r="O942">
+        <v>79</v>
+      </c>
+      <c r="P942">
+        <v>55</v>
       </c>
     </row>
     <row r="943" spans="1:20" x14ac:dyDescent="0.35">
@@ -86080,19 +86170,55 @@
         <v>58</v>
       </c>
       <c r="C943" t="s">
-        <v>1120</v>
+        <v>1133</v>
       </c>
       <c r="D943">
         <v>4</v>
       </c>
       <c r="E943" t="s">
-        <v>1220</v>
+        <v>1230</v>
       </c>
       <c r="F943">
         <v>2</v>
       </c>
       <c r="G943">
         <v>6</v>
+      </c>
+      <c r="H943">
+        <v>88</v>
+      </c>
+      <c r="I943">
+        <v>76</v>
+      </c>
+      <c r="J943">
+        <v>94</v>
+      </c>
+      <c r="K943">
+        <v>71</v>
+      </c>
+      <c r="L943">
+        <v>65</v>
+      </c>
+      <c r="M943">
+        <v>77</v>
+      </c>
+      <c r="O943">
+        <v>84</v>
+      </c>
+      <c r="P943">
+        <v>62</v>
+      </c>
+      <c r="Q943">
+        <v>74</v>
+      </c>
+      <c r="R943">
+        <v>83</v>
+      </c>
+      <c r="S943">
+        <v>74</v>
+      </c>
+      <c r="T943">
+        <v>56</v>
       </c>
     </row>
     <row r="944" spans="1:20" x14ac:dyDescent="0.35">
@@ -86103,19 +86229,37 @@
         <v>1231</v>
       </c>
       <c r="C944" t="s">
-        <v>1079</v>
+        <v>1228</v>
       </c>
       <c r="D944">
         <v>2</v>
       </c>
       <c r="E944" t="s">
-        <v>308</v>
+        <v>1143</v>
       </c>
       <c r="F944">
         <v>1</v>
       </c>
       <c r="G944">
         <v>3</v>
+      </c>
+      <c r="H944">
+        <v>85</v>
+      </c>
+      <c r="I944">
+        <v>69</v>
+      </c>
+      <c r="J944">
+        <v>84</v>
+      </c>
+      <c r="O944">
+        <v>81</v>
+      </c>
+      <c r="P944">
+        <v>79</v>
+      </c>
+      <c r="Q944">
+        <v>77</v>
       </c>
     </row>
     <row r="945" spans="1:21" x14ac:dyDescent="0.35">
@@ -86126,19 +86270,37 @@
         <v>1231</v>
       </c>
       <c r="C945" t="s">
-        <v>1221</v>
+        <v>1196</v>
       </c>
       <c r="D945">
         <v>2</v>
       </c>
       <c r="E945" t="s">
-        <v>151</v>
+        <v>1260</v>
       </c>
       <c r="F945">
         <v>1</v>
       </c>
       <c r="G945">
         <v>3</v>
+      </c>
+      <c r="H945">
+        <v>79</v>
+      </c>
+      <c r="I945">
+        <v>77</v>
+      </c>
+      <c r="J945">
+        <v>81</v>
+      </c>
+      <c r="O945">
+        <v>72</v>
+      </c>
+      <c r="P945">
+        <v>81</v>
+      </c>
+      <c r="Q945">
+        <v>74</v>
       </c>
     </row>
     <row r="946" spans="1:21" x14ac:dyDescent="0.35">
@@ -86149,19 +86311,31 @@
         <v>1214</v>
       </c>
       <c r="C946" t="s">
-        <v>1079</v>
+        <v>1228</v>
       </c>
       <c r="D946">
         <v>2</v>
       </c>
       <c r="E946" t="s">
-        <v>1221</v>
+        <v>1196</v>
       </c>
       <c r="F946">
         <v>0</v>
       </c>
       <c r="G946">
         <v>2</v>
+      </c>
+      <c r="H946">
+        <v>73</v>
+      </c>
+      <c r="I946">
+        <v>89</v>
+      </c>
+      <c r="O946">
+        <v>67</v>
+      </c>
+      <c r="P946">
+        <v>72</v>
       </c>
     </row>
     <row r="947" spans="1:21" x14ac:dyDescent="0.35">
@@ -86172,13 +86346,13 @@
         <v>1214</v>
       </c>
       <c r="C947" t="s">
-        <v>1148</v>
+        <v>1259</v>
       </c>
       <c r="D947">
         <v>4</v>
       </c>
       <c r="E947" t="s">
-        <v>1236</v>
+        <v>1322</v>
       </c>
       <c r="F947">
         <v>3</v>
@@ -86237,19 +86411,55 @@
         <v>58</v>
       </c>
       <c r="C948" t="s">
-        <v>1079</v>
+        <v>1228</v>
       </c>
       <c r="D948">
         <v>4</v>
       </c>
       <c r="E948" t="s">
-        <v>1148</v>
+        <v>1259</v>
       </c>
       <c r="F948">
         <v>2</v>
       </c>
       <c r="G948">
         <v>6</v>
+      </c>
+      <c r="H948">
+        <v>60</v>
+      </c>
+      <c r="I948">
+        <v>66</v>
+      </c>
+      <c r="J948">
+        <v>72</v>
+      </c>
+      <c r="K948">
+        <v>78</v>
+      </c>
+      <c r="L948">
+        <v>82</v>
+      </c>
+      <c r="M948">
+        <v>88</v>
+      </c>
+      <c r="O948">
+        <v>71</v>
+      </c>
+      <c r="P948">
+        <v>63</v>
+      </c>
+      <c r="Q948">
+        <v>70</v>
+      </c>
+      <c r="R948">
+        <v>75</v>
+      </c>
+      <c r="S948">
+        <v>91</v>
+      </c>
+      <c r="T948">
+        <v>73</v>
       </c>
     </row>
     <row r="949" spans="1:21" x14ac:dyDescent="0.35">
@@ -86260,19 +86470,37 @@
         <v>1231</v>
       </c>
       <c r="C949" t="s">
-        <v>555</v>
+        <v>1143</v>
       </c>
       <c r="D949">
         <v>2</v>
       </c>
       <c r="E949" t="s">
-        <v>1239</v>
+        <v>1323</v>
       </c>
       <c r="F949">
         <v>1</v>
       </c>
       <c r="G949">
         <v>3</v>
+      </c>
+      <c r="H949">
+        <v>51</v>
+      </c>
+      <c r="I949">
+        <v>86</v>
+      </c>
+      <c r="J949">
+        <v>93</v>
+      </c>
+      <c r="O949">
+        <v>77</v>
+      </c>
+      <c r="P949">
+        <v>74</v>
+      </c>
+      <c r="Q949">
+        <v>71</v>
       </c>
     </row>
     <row r="950" spans="1:21" x14ac:dyDescent="0.35">
@@ -86283,19 +86511,37 @@
         <v>1231</v>
       </c>
       <c r="C950" t="s">
-        <v>1101</v>
+        <v>1259</v>
       </c>
       <c r="D950">
         <v>2</v>
       </c>
       <c r="E950" t="s">
-        <v>1241</v>
+        <v>1322</v>
       </c>
       <c r="F950">
         <v>1</v>
       </c>
       <c r="G950">
         <v>3</v>
+      </c>
+      <c r="H950">
+        <v>73</v>
+      </c>
+      <c r="I950">
+        <v>51</v>
+      </c>
+      <c r="J950">
+        <v>75</v>
+      </c>
+      <c r="O950">
+        <v>68</v>
+      </c>
+      <c r="P950">
+        <v>73</v>
+      </c>
+      <c r="Q950">
+        <v>59</v>
       </c>
     </row>
     <row r="951" spans="1:21" x14ac:dyDescent="0.35">
@@ -86306,19 +86552,55 @@
         <v>1214</v>
       </c>
       <c r="C951" t="s">
-        <v>1243</v>
+        <v>1196</v>
       </c>
       <c r="D951">
         <v>4</v>
       </c>
       <c r="E951" t="s">
-        <v>1220</v>
+        <v>1230</v>
       </c>
       <c r="F951">
         <v>2</v>
       </c>
       <c r="G951">
         <v>6</v>
+      </c>
+      <c r="H951">
+        <v>81</v>
+      </c>
+      <c r="I951">
+        <v>69</v>
+      </c>
+      <c r="J951">
+        <v>67</v>
+      </c>
+      <c r="K951">
+        <v>69</v>
+      </c>
+      <c r="L951">
+        <v>55</v>
+      </c>
+      <c r="M951">
+        <v>66</v>
+      </c>
+      <c r="O951">
+        <v>65</v>
+      </c>
+      <c r="P951">
+        <v>53</v>
+      </c>
+      <c r="Q951">
+        <v>55</v>
+      </c>
+      <c r="R951">
+        <v>76</v>
+      </c>
+      <c r="S951">
+        <v>67</v>
+      </c>
+      <c r="T951">
+        <v>61</v>
       </c>
     </row>
     <row r="952" spans="1:21" x14ac:dyDescent="0.35">
@@ -86329,19 +86611,31 @@
         <v>1214</v>
       </c>
       <c r="C952" t="s">
-        <v>1101</v>
+        <v>1259</v>
       </c>
       <c r="D952">
         <v>2</v>
       </c>
       <c r="E952" t="s">
-        <v>555</v>
+        <v>1143</v>
       </c>
       <c r="F952">
         <v>0</v>
       </c>
       <c r="G952">
         <v>2</v>
+      </c>
+      <c r="H952">
+        <v>82</v>
+      </c>
+      <c r="I952">
+        <v>72</v>
+      </c>
+      <c r="O952">
+        <v>70</v>
+      </c>
+      <c r="P952">
+        <v>53</v>
       </c>
     </row>
     <row r="953" spans="1:21" x14ac:dyDescent="0.35">
@@ -86352,19 +86646,49 @@
         <v>58</v>
       </c>
       <c r="C953" t="s">
-        <v>1101</v>
+        <v>1259</v>
       </c>
       <c r="D953">
         <v>4</v>
       </c>
       <c r="E953" t="s">
-        <v>1243</v>
+        <v>1196</v>
       </c>
       <c r="F953">
         <v>1</v>
       </c>
       <c r="G953">
         <v>5</v>
+      </c>
+      <c r="H953">
+        <v>84</v>
+      </c>
+      <c r="I953">
+        <v>85</v>
+      </c>
+      <c r="J953">
+        <v>75</v>
+      </c>
+      <c r="K953">
+        <v>73</v>
+      </c>
+      <c r="L953">
+        <v>83</v>
+      </c>
+      <c r="O953">
+        <v>71</v>
+      </c>
+      <c r="P953">
+        <v>74</v>
+      </c>
+      <c r="Q953">
+        <v>72</v>
+      </c>
+      <c r="R953">
+        <v>74</v>
+      </c>
+      <c r="S953">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add point differences computation and output to data pipeline. Compute weights with new dataset
</commit_message>
<xml_diff>
--- a/NBASeriesML/NBASeriesResults.xlsx
+++ b/NBASeriesML/NBASeriesResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usolon\Documents\NBASeriesML\NBASeriesML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03765E68-1865-4863-B9DF-0F6CD690DAD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C8C18C5-A2F2-4B30-BFB0-E32662D26F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{E5EB9399-3DE7-464A-8398-E490882B2270}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{E5EB9399-3DE7-464A-8398-E490882B2270}"/>
   </bookViews>
   <sheets>
     <sheet name="NBASeriesResults_v2025" sheetId="3" r:id="rId1"/>
@@ -1345,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDB2D06D-6BBD-46A2-823D-1E442DB84DAE}">
   <dimension ref="A1:V953"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -55227,7 +55227,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F409A88-CE45-4166-B2ED-8A0292BD5E60}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>

</xml_diff>